<commit_message>
Subiendo nuevo test_register y locator de register y maqueta de login
</commit_message>
<xml_diff>
--- a/tests/files/files_data_source/registros_exitosos.xlsx
+++ b/tests/files/files_data_source/registros_exitosos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,30 +424,35 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>baezajuliana249</t>
+          <t>adelina41736</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Eutimio</t>
+          <t>Maricruz</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Molins</t>
+          <t>Zamora</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>carreteroclara@alcantara.com</t>
+          <t>igalindo@gmail.com</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>P9F$S*mx+j(N</t>
+          <t>W5V&amp;vdsE0LHZ</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
+        <is>
+          <t>W5V&amp;vdsE0LHZ</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>Válido</t>
         </is>
@@ -456,30 +461,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ynavarro356</t>
+          <t>samanta15396</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Juana</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alarcón</t>
+          <t>Silva</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>mariscalaurelio@yahoo.com</t>
+          <t>flastra@inversiones.es</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>p(W^mdu_&amp;)8G</t>
+          <t>m7FUa5ed*CIF</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>m7FUa5ed*CIF</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Válido</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>maciassarita605</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Elena</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Solana</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>emilia67@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2Tq(uBue#^o1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2Tq(uBue#^o1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Válido</t>
         </is>

</xml_diff>

<commit_message>
Subiendo ajuste en test_register
</commit_message>
<xml_diff>
--- a/tests/files/files_data_source/registros_exitosos.xlsx
+++ b/tests/files/files_data_source/registros_exitosos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,6 +532,43 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>lermacasemiro979</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Luz</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Macías</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>chita77@compania.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>#r(5dVgl)Cd2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>#r(5dVgl)Cd2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Válido</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajuste para guardar evidencia en nueva subcarpeta por cada tipo
</commit_message>
<xml_diff>
--- a/tests/files/files_data_source/registros_exitosos.xlsx
+++ b/tests/files/files_data_source/registros_exitosos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,43 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>tsolera656</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Raimundo</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Guijarro</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pmanjon@gmail.com</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>n^s4O8bE*z0m</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>n^s4O8bE*z0m</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Válido</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>